<commit_message>
pushign the changes doen for the failures in jenkins-Shaheena
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Login functionality.xlsx
+++ b/src/test/java/com/born/xls/Login functionality.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3015" tabRatio="652"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6795" tabRatio="652"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="87">
   <si>
     <t>TCID</t>
   </si>
@@ -265,22 +265,19 @@
     <t>col|UserName</t>
   </si>
   <si>
-    <t>DeltaFaucet7</t>
-  </si>
-  <si>
-    <t>Test7</t>
-  </si>
-  <si>
-    <t>DeltaFaucet7@gmail.com</t>
-  </si>
-  <si>
-    <t>Result1</t>
-  </si>
-  <si>
-    <t>FAIL -- Not able to navigate</t>
-  </si>
-  <si>
-    <t>FAIL -- text not verified  -- DeltaFaucet7</t>
+    <t>PASS -- text verified DeltaFaucet7 -- DeltaFaucet7</t>
+  </si>
+  <si>
+    <t>DeltaFaucet8</t>
+  </si>
+  <si>
+    <t>Test8</t>
+  </si>
+  <si>
+    <t>DeltaFaucet2@gmail.com</t>
+  </si>
+  <si>
+    <t>DeltaFaucet8@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -353,7 +350,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -402,11 +399,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -436,7 +428,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -464,7 +456,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -824,10 +815,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,11 +830,11 @@
     <col min="5" max="5" width="36.28515625" style="2" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="24.140625" style="2" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="20.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="8" max="9" width="9.140625" style="2"/>
+    <col min="10" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -865,11 +856,8 @@
       <c r="G1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>30</v>
       </c>
@@ -887,11 +875,8 @@
         <v>7</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
@@ -909,11 +894,8 @@
         <v>9</v>
       </c>
       <c r="G3" s="6"/>
-      <c r="H3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>30</v>
       </c>
@@ -931,11 +913,8 @@
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
@@ -953,11 +932,8 @@
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -977,11 +953,8 @@
         <v>31</v>
       </c>
       <c r="G6" s="6"/>
-      <c r="H6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -1001,11 +974,8 @@
         <v>32</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
@@ -1025,11 +995,8 @@
         <v>44</v>
       </c>
       <c r="G8" s="6"/>
-      <c r="H8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
@@ -1049,11 +1016,8 @@
         <v>29</v>
       </c>
       <c r="G9" s="6"/>
-      <c r="H9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
@@ -1073,11 +1037,8 @@
         <v>29</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="H10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>30</v>
       </c>
@@ -1095,11 +1056,8 @@
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>30</v>
       </c>
@@ -1117,11 +1075,8 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>30</v>
       </c>
@@ -1139,11 +1094,8 @@
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>30</v>
       </c>
@@ -1159,11 +1111,8 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1172,7 +1121,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>46</v>
       </c>
@@ -1190,11 +1139,8 @@
         <v>7</v>
       </c>
       <c r="G16" s="6"/>
-      <c r="H16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
@@ -1212,11 +1158,8 @@
         <v>9</v>
       </c>
       <c r="G17" s="6"/>
-      <c r="H17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>46</v>
       </c>
@@ -1234,11 +1177,8 @@
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>46</v>
       </c>
@@ -1258,11 +1198,8 @@
         <v>44</v>
       </c>
       <c r="G19" s="6"/>
-      <c r="H19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>46</v>
       </c>
@@ -1282,11 +1219,8 @@
         <v>29</v>
       </c>
       <c r="G20" s="6"/>
-      <c r="H20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>46</v>
       </c>
@@ -1304,11 +1238,8 @@
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>46</v>
       </c>
@@ -1328,11 +1259,8 @@
         <v>81</v>
       </c>
       <c r="G22" s="6"/>
-      <c r="H22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>46</v>
       </c>
@@ -1350,11 +1278,8 @@
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-      <c r="H23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>46</v>
       </c>
@@ -1372,11 +1297,8 @@
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>46</v>
       </c>
@@ -1394,11 +1316,8 @@
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>46</v>
       </c>
@@ -1414,9 +1333,6 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" t="s">
-        <v>75</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1429,7 +1345,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,7 +1355,7 @@
     <col min="3" max="3" width="28.140625" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="24.85546875" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -1464,13 +1380,13 @@
     </row>
     <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>42</v>
@@ -1479,7 +1395,7 @@
         <v>58</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1495,7 +1411,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1419,7 @@
     <col min="1" max="1" width="13.85546875" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="45" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1525,10 +1441,10 @@
     </row>
     <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>42</v>
@@ -1537,7 +1453,7 @@
         <v>58</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commiting the latest changes done by shaheena
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Login functionality.xlsx
+++ b/src/test/java/com/born/xls/Login functionality.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6795" tabRatio="652"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3015" tabRatio="652"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="77">
   <si>
     <t>TCID</t>
   </si>
@@ -112,18 +112,6 @@
     <t>Registration</t>
   </si>
   <si>
-    <t>col|FirstName</t>
-  </si>
-  <si>
-    <t>col|LastName</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
     <t>Enter the FirstName</t>
   </si>
   <si>
@@ -244,9 +232,6 @@
     <t>Register_Message</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>LoggedIn_UserName_Text</t>
   </si>
   <si>
@@ -256,28 +241,13 @@
     <t>Click on Logged-in username</t>
   </si>
   <si>
-    <t>ContainsText</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>col|UserName</t>
-  </si>
-  <si>
-    <t>PASS -- text verified DeltaFaucet7 -- DeltaFaucet7</t>
-  </si>
-  <si>
-    <t>DeltaFaucet8</t>
-  </si>
-  <si>
-    <t>Test8</t>
-  </si>
-  <si>
-    <t>DeltaFaucet2@gmail.com</t>
-  </si>
-  <si>
-    <t>DeltaFaucet8@gmail.com</t>
+    <t>RegisterEmail</t>
+  </si>
+  <si>
+    <t>DeltaFaucet9@gmail.com</t>
+  </si>
+  <si>
+    <t>RandomString</t>
   </si>
 </sst>
 </file>
@@ -428,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -455,7 +425,6 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -764,7 +733,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,21 +760,21 @@
         <v>30</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -815,10 +784,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,8 +799,8 @@
     <col min="5" max="5" width="36.28515625" style="2" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="24.140625" style="2" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="20.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="9.140625" style="2"/>
-    <col min="10" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="8" max="8" width="9.140625" style="2"/>
+    <col min="9" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -865,7 +834,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>26</v>
@@ -906,10 +875,10 @@
         <v>27</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -922,13 +891,13 @@
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -941,17 +910,15 @@
         <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>31</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -962,17 +929,15 @@
         <v>16</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>32</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -983,17 +948,15 @@
         <v>17</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>44</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1001,16 +964,16 @@
         <v>30</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>29</v>
@@ -1025,13 +988,13 @@
         <v>23</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>29</v>
@@ -1046,13 +1009,13 @@
         <v>18</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -1065,13 +1028,13 @@
         <v>19</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -1084,13 +1047,13 @@
         <v>20</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -1103,10 +1066,10 @@
         <v>22</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -1123,13 +1086,13 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>26</v>
@@ -1142,7 +1105,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>12</v>
@@ -1161,7 +1124,7 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>13</v>
@@ -1170,44 +1133,44 @@
         <v>27</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>10</v>
@@ -1222,113 +1185,111 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="E22" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>81</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="F22" s="13"/>
       <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
@@ -1342,123 +1303,88 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>75</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C2" s="9"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="DeltaFaucet@gmail.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="36" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>80</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>82</v>
-      </c>
+    <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="DeltaFaucet@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="DeltaFaucet@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
pushing the chnages done by shaheena 1) changed keywords in sheets 2)changed the testcases position
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Login functionality.xlsx
+++ b/src/test/java/com/born/xls/Login functionality.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3015" tabRatio="652"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3010" tabRatio="652" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -398,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -411,6 +411,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -730,21 +731,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="64.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" width="23.81640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="64.7265625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.7265625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.1796875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -755,27 +756,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.4">
+      <c r="A2" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.4">
+      <c r="A3" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>54</v>
       </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.4">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -787,23 +793,23 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.140625" style="2" collapsed="1"/>
-    <col min="3" max="3" width="47.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
-    <col min="9" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" width="14.36328125" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.1796875" style="2" collapsed="1"/>
+    <col min="3" max="3" width="47.1796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.7265625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.26953125" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.1796875" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.54296875" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.1796875" style="2"/>
+    <col min="9" max="16384" width="9.1796875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -826,7 +832,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>30</v>
       </c>
@@ -845,7 +851,7 @@
       </c>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
@@ -864,7 +870,7 @@
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>30</v>
       </c>
@@ -883,7 +889,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
@@ -902,7 +908,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -921,7 +927,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -940,7 +946,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
@@ -959,7 +965,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
@@ -980,7 +986,7 @@
       </c>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
@@ -1001,7 +1007,7 @@
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>30</v>
       </c>
@@ -1020,7 +1026,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>30</v>
       </c>
@@ -1039,7 +1045,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>30</v>
       </c>
@@ -1058,7 +1064,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>30</v>
       </c>
@@ -1075,7 +1081,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1084,7 +1090,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>42</v>
       </c>
@@ -1103,7 +1109,7 @@
       </c>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>42</v>
       </c>
@@ -1116,13 +1122,13 @@
       <c r="D17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="11"/>
+      <c r="E17" s="12"/>
       <c r="F17" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
@@ -1141,7 +1147,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>42</v>
       </c>
@@ -1162,7 +1168,7 @@
       </c>
       <c r="G19" s="6"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>42</v>
       </c>
@@ -1183,7 +1189,7 @@
       </c>
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>42</v>
       </c>
@@ -1202,7 +1208,7 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>42</v>
       </c>
@@ -1218,10 +1224,10 @@
       <c r="E22" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F22" s="13"/>
+      <c r="F22" s="14"/>
       <c r="G22" s="6"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>42</v>
       </c>
@@ -1240,7 +1246,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>42</v>
       </c>
@@ -1259,7 +1265,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>42</v>
       </c>
@@ -1278,7 +1284,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>42</v>
       </c>
@@ -1309,32 +1315,32 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.81640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.4">
+      <c r="A1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.4">
+      <c r="A2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1345,18 +1351,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.81640625" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="36" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
@@ -1370,11 +1376,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.4">
+      <c r="A2" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C2" s="4" t="s">

</xml_diff>

<commit_message>
pushing the changes done by shaheena 12/02
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Login functionality.xlsx
+++ b/src/test/java/com/born/xls/Login functionality.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3010" tabRatio="652" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3010" tabRatio="652"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -733,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1351,7 +1351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes has done for failure TC
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Login functionality.xlsx
+++ b/src/test/java/com/born/xls/Login functionality.xlsx
@@ -398,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -411,7 +411,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -731,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -757,31 +756,26 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1122,7 +1116,7 @@
       <c r="D17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="12"/>
+      <c r="E17" s="11"/>
       <c r="F17" s="6" t="s">
         <v>9</v>
       </c>
@@ -1224,7 +1218,7 @@
       <c r="E22" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F22" s="14"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1323,24 +1317,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1377,10 +1371,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.4">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>38</v>
       </c>
       <c r="C2" s="4" t="s">

</xml_diff>

<commit_message>
Modified excel sheet name from MyAccount to PLP, since all tc's related to plp page.
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Login functionality.xlsx
+++ b/src/test/java/com/born/xls/Login functionality.xlsx
@@ -786,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1306,7 +1306,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1346,14 +1346,14 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.7265625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="17.81640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="36" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.36328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Segregated and added one more excel sheet accordingly test cases functionality.
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Login functionality.xlsx
+++ b/src/test/java/com/born/xls/Login functionality.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3010" tabRatio="652"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3010" tabRatio="652" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="79">
   <si>
     <t>TCID</t>
   </si>
@@ -184,9 +184,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Verify the user is bale to login succefully</t>
-  </si>
-  <si>
     <t>Verify the user can Register for an account successfully</t>
   </si>
   <si>
@@ -248,6 +245,15 @@
   </si>
   <si>
     <t>RandomString</t>
+  </si>
+  <si>
+    <t>Result1</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Verify the user is abale to login succefully</t>
   </si>
 </sst>
 </file>
@@ -320,7 +326,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,6 +375,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -398,7 +409,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -425,6 +436,7 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -732,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -760,7 +772,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>54</v>
@@ -771,7 +783,7 @@
         <v>42</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>54</v>
@@ -786,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -799,11 +811,11 @@
     <col min="5" max="5" width="36.26953125" style="2" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="24.1796875" style="2" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="20.54296875" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.1796875" style="2"/>
+    <col min="8" max="8" width="7.54296875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="16384" width="9.1796875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -825,8 +837,11 @@
       <c r="G1" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H1" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>30</v>
       </c>
@@ -844,8 +859,11 @@
         <v>7</v>
       </c>
       <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
@@ -863,8 +881,11 @@
         <v>9</v>
       </c>
       <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>30</v>
       </c>
@@ -878,12 +899,15 @@
         <v>35</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
@@ -897,12 +921,15 @@
         <v>35</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -913,15 +940,18 @@
         <v>31</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -932,15 +962,18 @@
         <v>32</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
@@ -951,15 +984,18 @@
         <v>33</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
@@ -973,14 +1009,17 @@
         <v>10</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>29</v>
       </c>
       <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
@@ -994,14 +1033,17 @@
         <v>10</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>29</v>
       </c>
       <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>30</v>
       </c>
@@ -1015,12 +1057,15 @@
         <v>35</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>30</v>
       </c>
@@ -1028,18 +1073,21 @@
         <v>19</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>30</v>
       </c>
@@ -1047,18 +1095,21 @@
         <v>20</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>51</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>30</v>
       </c>
@@ -1066,7 +1117,7 @@
         <v>22</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>53</v>
@@ -1074,8 +1125,11 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1084,7 +1138,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>42</v>
       </c>
@@ -1102,8 +1156,11 @@
         <v>7</v>
       </c>
       <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>42</v>
       </c>
@@ -1121,8 +1178,11 @@
         <v>9</v>
       </c>
       <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
@@ -1136,12 +1196,15 @@
         <v>35</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>42</v>
       </c>
@@ -1155,14 +1218,17 @@
         <v>10</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>40</v>
       </c>
       <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>42</v>
       </c>
@@ -1182,8 +1248,11 @@
         <v>29</v>
       </c>
       <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>42</v>
       </c>
@@ -1197,12 +1266,15 @@
         <v>35</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>42</v>
       </c>
@@ -1216,12 +1288,15 @@
         <v>51</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F22" s="13"/>
       <c r="G22" s="6"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>42</v>
       </c>
@@ -1229,18 +1304,21 @@
         <v>36</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>35</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>42</v>
       </c>
@@ -1254,12 +1332,15 @@
         <v>35</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>42</v>
       </c>
@@ -1273,12 +1354,15 @@
         <v>51</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>42</v>
       </c>
@@ -1294,6 +1378,9 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
+      <c r="H26" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1334,7 +1421,9 @@
       <c r="B2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="9" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1345,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1372,7 +1461,7 @@
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>38</v>
@@ -1380,7 +1469,9 @@
       <c r="C2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Modified object for failed tc
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Login functionality.xlsx
+++ b/src/test/java/com/born/xls/Login functionality.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="77">
   <si>
     <t>TCID</t>
   </si>
@@ -245,12 +245,6 @@
   </si>
   <si>
     <t>RandomString</t>
-  </si>
-  <si>
-    <t>Result1</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
   <si>
     <t>Verify the user is abale to login succefully</t>
@@ -326,7 +320,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -375,11 +369,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -409,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -436,7 +425,6 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -783,7 +771,7 @@
         <v>42</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>54</v>
@@ -796,10 +784,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -811,11 +799,12 @@
     <col min="5" max="5" width="36.26953125" style="2" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="24.1796875" style="2" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="20.54296875" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.54296875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.1796875" style="2" collapsed="1"/>
+    <col min="8" max="8" width="9.1796875" style="2" collapsed="1"/>
+    <col min="9" max="9" width="9.1796875" style="2"/>
+    <col min="10" max="16384" width="9.1796875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -837,11 +826,8 @@
       <c r="G1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>30</v>
       </c>
@@ -859,11 +845,8 @@
         <v>7</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
@@ -881,11 +864,8 @@
         <v>9</v>
       </c>
       <c r="G3" s="6"/>
-      <c r="H3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>30</v>
       </c>
@@ -903,11 +883,8 @@
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
@@ -925,11 +902,8 @@
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -947,11 +921,8 @@
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
@@ -969,11 +940,8 @@
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
@@ -991,11 +959,8 @@
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
@@ -1015,11 +980,8 @@
         <v>29</v>
       </c>
       <c r="G9" s="6"/>
-      <c r="H9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
@@ -1039,11 +1001,8 @@
         <v>29</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="H10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>30</v>
       </c>
@@ -1061,11 +1020,8 @@
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>30</v>
       </c>
@@ -1083,11 +1039,8 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>30</v>
       </c>
@@ -1105,11 +1058,8 @@
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>30</v>
       </c>
@@ -1125,11 +1075,8 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1138,7 +1085,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>42</v>
       </c>
@@ -1156,11 +1103,8 @@
         <v>7</v>
       </c>
       <c r="G16" s="6"/>
-      <c r="H16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>42</v>
       </c>
@@ -1178,11 +1122,8 @@
         <v>9</v>
       </c>
       <c r="G17" s="6"/>
-      <c r="H17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
@@ -1200,11 +1141,8 @@
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>42</v>
       </c>
@@ -1224,11 +1162,8 @@
         <v>40</v>
       </c>
       <c r="G19" s="6"/>
-      <c r="H19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>42</v>
       </c>
@@ -1248,11 +1183,8 @@
         <v>29</v>
       </c>
       <c r="G20" s="6"/>
-      <c r="H20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>42</v>
       </c>
@@ -1270,11 +1202,8 @@
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>42</v>
       </c>
@@ -1292,11 +1221,8 @@
       </c>
       <c r="F22" s="13"/>
       <c r="G22" s="6"/>
-      <c r="H22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>42</v>
       </c>
@@ -1314,11 +1240,8 @@
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-      <c r="H23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>42</v>
       </c>
@@ -1336,11 +1259,8 @@
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>42</v>
       </c>
@@ -1358,11 +1278,8 @@
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>42</v>
       </c>
@@ -1378,9 +1295,6 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" t="s">
-        <v>77</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1421,9 +1335,7 @@
       <c r="B2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>77</v>
-      </c>
+      <c r="C2" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1435,7 +1347,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1469,9 +1381,7 @@
       <c r="C2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>77</v>
-      </c>
+      <c r="D2" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added Product Registration TC
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Login functionality.xlsx
+++ b/src/test/java/com/born/xls/Login functionality.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3010" tabRatio="652" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3010" tabRatio="652" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -786,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1346,7 +1346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Executing the TC's  in Firefox browser
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Login functionality.xlsx
+++ b/src/test/java/com/born/xls/Login functionality.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3010" tabRatio="652" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3010" tabRatio="652" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -733,7 +733,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -784,10 +784,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -799,9 +799,9 @@
     <col min="5" max="5" width="36.26953125" style="2" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="24.1796875" style="2" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="20.54296875" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.1796875" style="2" collapsed="1"/>
-    <col min="9" max="9" width="9.1796875" style="2"/>
-    <col min="10" max="16384" width="9.1796875" style="2" collapsed="1"/>
+    <col min="8" max="9" width="9.1796875" style="2" collapsed="1"/>
+    <col min="10" max="10" width="9.1796875" style="2"/>
+    <col min="11" max="16384" width="9.1796875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1346,7 +1346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated working code in chrome and firefox
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Login functionality.xlsx
+++ b/src/test/java/com/born/xls/Login functionality.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3010" tabRatio="652" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3010" tabRatio="652" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="78">
   <si>
     <t>TCID</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>Verify the user is abale to login succefully</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -784,10 +787,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -799,9 +802,9 @@
     <col min="5" max="5" width="36.26953125" style="2" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="24.1796875" style="2" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="20.54296875" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="9.1796875" style="2" collapsed="1"/>
-    <col min="10" max="10" width="9.1796875" style="2"/>
-    <col min="11" max="16384" width="9.1796875" style="2" collapsed="1"/>
+    <col min="8" max="11" width="9.1796875" style="2" collapsed="1"/>
+    <col min="12" max="12" width="9.1796875" style="2"/>
+    <col min="13" max="16384" width="9.1796875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1307,7 +1310,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1335,7 +1338,9 @@
       <c r="B2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="9" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1346,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1381,7 +1386,9 @@
       <c r="C2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
pushing the changes done for Deltafaucet.
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Login functionality.xlsx
+++ b/src/test/java/com/born/xls/Login functionality.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3010" tabRatio="652" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3010" tabRatio="652"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="79">
   <si>
     <t>TCID</t>
   </si>
@@ -251,13 +251,17 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>Result1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,7 +327,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,6 +376,16 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -401,7 +415,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -428,6 +442,7 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -735,16 +750,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.81640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="64.7265625" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.7265625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.1796875" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="23.81640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="64.7265625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="10.7265625" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -789,22 +804,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.1796875" style="2" collapsed="1"/>
-    <col min="3" max="3" width="47.1796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.7265625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.26953125" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.1796875" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.54296875" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="11" width="9.1796875" style="2" collapsed="1"/>
-    <col min="12" max="12" width="9.1796875" style="2"/>
-    <col min="13" max="16384" width="9.1796875" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="14.36328125" collapsed="true"/>
+    <col min="2" max="2" style="2" width="9.1796875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="47.1796875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="26.7265625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="36.26953125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="24.1796875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="20.54296875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="9" max="11" style="2" width="9.1796875" collapsed="true"/>
+    <col min="12" max="12" style="2" width="9.1796875" collapsed="true"/>
+    <col min="13" max="16384" style="2" width="9.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -829,6 +845,9 @@
       <c r="G1" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="H1" t="s" s="14">
+        <v>78</v>
+      </c>
     </row>
     <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -848,6 +867,9 @@
         <v>7</v>
       </c>
       <c r="G2" s="6"/>
+      <c r="H2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
@@ -867,6 +889,9 @@
         <v>9</v>
       </c>
       <c r="G3" s="6"/>
+      <c r="H3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
@@ -886,6 +911,9 @@
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
+      <c r="H4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
@@ -905,6 +933,9 @@
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
+      <c r="H5" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
@@ -924,6 +955,9 @@
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
+      <c r="H6" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
@@ -943,6 +977,9 @@
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
+      <c r="H7" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
@@ -962,6 +999,9 @@
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
+      <c r="H8" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
@@ -983,6 +1023,9 @@
         <v>29</v>
       </c>
       <c r="G9" s="6"/>
+      <c r="H9" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
@@ -1004,6 +1047,9 @@
         <v>29</v>
       </c>
       <c r="G10" s="6"/>
+      <c r="H10" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
@@ -1023,6 +1069,9 @@
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
+      <c r="H11" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
@@ -1042,6 +1091,9 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
+      <c r="H12" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
@@ -1061,6 +1113,9 @@
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
+      <c r="H13" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
@@ -1078,6 +1133,9 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
+      <c r="H14" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
@@ -1106,6 +1164,9 @@
         <v>7</v>
       </c>
       <c r="G16" s="6"/>
+      <c r="H16" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
@@ -1125,6 +1186,9 @@
         <v>9</v>
       </c>
       <c r="G17" s="6"/>
+      <c r="H17" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
@@ -1144,6 +1208,9 @@
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
+      <c r="H18" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
@@ -1165,6 +1232,9 @@
         <v>40</v>
       </c>
       <c r="G19" s="6"/>
+      <c r="H19" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
@@ -1186,6 +1256,9 @@
         <v>29</v>
       </c>
       <c r="G20" s="6"/>
+      <c r="H20" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
@@ -1205,6 +1278,9 @@
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
+      <c r="H21" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
@@ -1224,6 +1300,9 @@
       </c>
       <c r="F22" s="13"/>
       <c r="G22" s="6"/>
+      <c r="H22" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
@@ -1243,6 +1322,9 @@
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
+      <c r="H23" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
@@ -1262,6 +1344,9 @@
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
+      <c r="H24" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
@@ -1281,6 +1366,9 @@
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
+      <c r="H25" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
@@ -1298,6 +1386,9 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
+      <c r="H26" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1315,9 +1406,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.81640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.81640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.5625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.4">
@@ -1357,9 +1448,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.81640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.7265625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.81640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.3984375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Removed Product Registration TC since they added captcha functionlaity.
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Login functionality.xlsx
+++ b/src/test/java/com/born/xls/Login functionality.xlsx
@@ -9,15 +9,14 @@
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Steps" sheetId="2" r:id="rId2"/>
-    <sheet name="Registration" sheetId="7" r:id="rId3"/>
-    <sheet name="Login" sheetId="8" r:id="rId4"/>
+    <sheet name="Login" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
   <si>
     <t>TCID</t>
   </si>
@@ -79,15 +78,9 @@
     <t>TS011</t>
   </si>
   <si>
-    <t>TS012</t>
-  </si>
-  <si>
     <t>Navigate to website</t>
   </si>
   <si>
-    <t>TS013</t>
-  </si>
-  <si>
     <t>TS009</t>
   </si>
   <si>
@@ -109,30 +102,12 @@
     <t>col|Password</t>
   </si>
   <si>
-    <t>Registration</t>
-  </si>
-  <si>
-    <t>Enter the FirstName</t>
-  </si>
-  <si>
-    <t>Enter the LastName</t>
-  </si>
-  <si>
-    <t>Enter the email address</t>
-  </si>
-  <si>
-    <t>Confirm the entered password</t>
-  </si>
-  <si>
     <t>enablehidden</t>
   </si>
   <si>
     <t>TS008</t>
   </si>
   <si>
-    <t>Select the Radio button</t>
-  </si>
-  <si>
     <t>DeltaFaucet@124</t>
   </si>
   <si>
@@ -142,9 +117,6 @@
     <t>col|Email</t>
   </si>
   <si>
-    <t>Enter the password</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
@@ -169,9 +141,6 @@
     <t>Open the browser</t>
   </si>
   <si>
-    <t>Click on the Register for an account button</t>
-  </si>
-  <si>
     <t>exist</t>
   </si>
   <si>
@@ -184,51 +153,15 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Verify the user can Register for an account successfully</t>
-  </si>
-  <si>
     <t>Login_btn</t>
   </si>
   <si>
-    <t>Register</t>
-  </si>
-  <si>
-    <t>First_name</t>
-  </si>
-  <si>
-    <t>Last_name</t>
-  </si>
-  <si>
-    <t>Click on Hamburge side menu</t>
-  </si>
-  <si>
     <t>sign-in</t>
   </si>
   <si>
-    <t>Re_type_pwd</t>
-  </si>
-  <si>
-    <t>Radio_Button</t>
-  </si>
-  <si>
-    <t>Submit</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
-    <t>Click on the Submit button</t>
-  </si>
-  <si>
-    <t>RegistorPassword</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Close the browser </t>
-  </si>
-  <si>
-    <t>Register_Message</t>
-  </si>
-  <si>
     <t>LoggedIn_UserName_Text</t>
   </si>
   <si>
@@ -238,30 +171,20 @@
     <t>Click on Logged-in username</t>
   </si>
   <si>
-    <t>RegisterEmail</t>
-  </si>
-  <si>
     <t>DeltaFaucet9@gmail.com</t>
   </si>
   <si>
-    <t>RandomString</t>
-  </si>
-  <si>
     <t>Verify the user is abale to login succefully</t>
   </si>
   <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>Result1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="9">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,13 +209,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -327,7 +243,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,24 +282,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill>
-        <fgColor indexed="55"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="55"/>
       </patternFill>
     </fill>
   </fills>
@@ -413,9 +313,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -426,23 +326,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -748,18 +643,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="23.81640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="64.7265625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="10.7265625" collapsed="true"/>
-    <col min="4" max="16384" style="2" width="9.1796875" collapsed="true"/>
+    <col min="1" max="1" width="23.81640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="64.7265625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.7265625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.1796875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -774,25 +669,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A2" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A3" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>54</v>
+      <c r="A2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -802,25 +686,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="14.36328125" collapsed="true"/>
-    <col min="2" max="2" style="2" width="9.1796875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="47.1796875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="26.7265625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="36.26953125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="2" width="24.1796875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="2" width="20.54296875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
-    <col min="9" max="11" style="2" width="9.1796875" collapsed="true"/>
-    <col min="12" max="12" style="2" width="9.1796875" collapsed="true"/>
-    <col min="13" max="16384" style="2" width="9.1796875" collapsed="true"/>
+    <col min="1" max="1" width="14.36328125" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.1796875" style="2" collapsed="1"/>
+    <col min="3" max="3" width="47.1796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.7265625" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.26953125" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.1796875" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.54296875" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.1796875" style="2" collapsed="1"/>
+    <col min="9" max="9" width="9.1796875" style="2"/>
+    <col min="10" max="16384" width="9.1796875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -843,552 +726,219 @@
         <v>6</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" t="s" s="14">
-        <v>78</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="9"/>
       <c r="F3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="6"/>
-      <c r="H3" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="G5" s="6"/>
-      <c r="H5" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="G6" s="6"/>
-      <c r="H6" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="6"/>
+        <v>49</v>
+      </c>
+      <c r="F8" s="11"/>
       <c r="G8" s="6"/>
-      <c r="H8" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>29</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>29</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>64</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="6"/>
-      <c r="H16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="6"/>
-      <c r="H17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="6"/>
-      <c r="H19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="6"/>
-      <c r="H20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="6"/>
-      <c r="H22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" t="s">
-        <v>77</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1398,87 +948,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.81640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.5625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.4">
-      <c r="A2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="24.7265625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="17.81640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="6.3984375" collapsed="true"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.81640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.36328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.4">
-      <c r="A2" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>38</v>
+      <c r="A2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Few New TC has been added.
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Login functionality.xlsx
+++ b/src/test/java/com/born/xls/Login functionality.xlsx
@@ -646,7 +646,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -686,10 +686,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -701,9 +701,9 @@
     <col min="5" max="5" width="36.26953125" style="2" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="24.1796875" style="2" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="20.54296875" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="9.1796875" style="2" collapsed="1"/>
-    <col min="10" max="10" width="9.1796875" style="2"/>
-    <col min="11" max="16384" width="9.1796875" style="2" collapsed="1"/>
+    <col min="8" max="8" width="9.1796875" style="2" collapsed="1"/>
+    <col min="9" max="9" width="9.1796875" style="2"/>
+    <col min="10" max="16384" width="9.1796875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Site Map has been modified according to prod env.
</commit_message>
<xml_diff>
--- a/src/test/java/com/born/xls/Login functionality.xlsx
+++ b/src/test/java/com/born/xls/Login functionality.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3010" tabRatio="652" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="3010" tabRatio="652"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView zoomScale="80" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>